<commit_message>
* [hunglv] Update Excel
</commit_message>
<xml_diff>
--- a/src/main/resources/ReportTemplate/Crewlist.xlsx
+++ b/src/main/resources/ReportTemplate/Crewlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <r>
       <rPr>
@@ -351,31 +351,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Số hộ chiếu PT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-Passport No.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve"> H</t>
     </r>
     <r>
@@ -542,6 +517,56 @@
       </rPr>
       <t xml:space="preserve">
  P.O.B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sổ TV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Seaman's book</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> H</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ộ chiếu TV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Passport No.</t>
     </r>
   </si>
 </sst>
@@ -760,15 +785,36 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -778,29 +824,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,7 +1212,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1215,14 +1240,14 @@
     <row r="2" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="C2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="14"/>
       <c r="J2" s="13"/>
       <c r="K2" s="13"/>
@@ -1232,7 +1257,7 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -1259,38 +1284,41 @@
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
+      <c r="A5" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
     </row>
     <row r="6" spans="1:13" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -1298,51 +1326,51 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="28"/>
+      <c r="J7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="23"/>
       <c r="L7" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="17" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="17" t="s">
+      <c r="F9" s="21"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="29" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="29" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
     </row>
     <row r="12" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1352,25 +1380,25 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>13</v>
@@ -1404,12 +1432,12 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
     </row>
@@ -1438,12 +1466,12 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
     </row>
@@ -1479,6 +1507,9 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A5:L6"/>
+    <mergeCell ref="H15:K15"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C9:D9"/>
@@ -1494,12 +1525,9 @@
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A5:L6"/>
-    <mergeCell ref="H15:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="79" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="79" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>